<commit_message>
clear the result data in data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>SearchString</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,16 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Allen_百度搜索</t>
-  </si>
-  <si>
-    <t>显示为 15</t>
   </si>
 </sst>
 </file>
@@ -571,7 +561,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -614,9 +604,6 @@
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
@@ -742,7 +729,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -788,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Add auto_api tc with 2kws
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WEB_UI" sheetId="1" r:id="rId1"/>
     <sheet name="WIN_UI" sheetId="2" r:id="rId2"/>
+    <sheet name="API_Get" sheetId="3" r:id="rId3"/>
+    <sheet name="API_Post" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>SearchString</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,14 +188,67 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>用例名/模块</t>
+  </si>
+  <si>
+    <t>base_url</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>reserve1</t>
+  </si>
+  <si>
+    <t>status_code</t>
+  </si>
+  <si>
+    <t>resp_body</t>
+  </si>
+  <si>
+    <t>结果回写</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Get_Official_Accounts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://wanandroid.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/wxarticle/chapters/json</t>
+  </si>
+  <si>
+    <t>{"data":[{"children":[],"courseId":13,"id":408,"name":"鸿洋","order":190000,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":409,"name":"郭霖","order":190001,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":410,"name":"玉刚说","order":190002,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":411,"name":"承香墨影","order":190003,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":413,"name":"Android群英传","order":190004,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":414,"name":"code小生","order":190005,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":415,"name":"谷歌开发者","order":190006,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":416,"name":"奇卓社","order":190007,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":417,"name":"美团技术团队","order":190008,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":420,"name":"GcsSloop","order":190009,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":421,"name":"互联网侦察","order":190010,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":427,"name":"susion随心","order":190011,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":428,"name":"程序亦非猿","order":190012,"parentChapterId":407,"userControlSetTop":false,"visible":1},{"children":[],"courseId":13,"id":434,"name":"Gityuan","order":190013,"parentChapterId":407,"userControlSetTop":false,"visible":1}],"errorCode":0,"errorMsg":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>req_body</t>
+  </si>
+  <si>
+    <t>关键字1校验</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,16 +272,73 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -260,11 +372,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,9 +430,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,12 +763,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.75" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.75" collapsed="true"/>
+    <col min="1" max="1" width="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.75" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -728,17 +925,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.75" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="1" max="1" width="13.625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -895,4 +1092,132 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
+    <col min="5" max="5" width="12.75" customWidth="1"/>
+    <col min="6" max="6" width="10.375" customWidth="1"/>
+    <col min="7" max="7" width="29.875" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="19.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>